<commit_message>
normalization logic, general updates
</commit_message>
<xml_diff>
--- a/input/administration_route/administration_route_to_curate_2021-08-26.xlsx
+++ b/input/administration_route/administration_route_to_curate_2021-08-26.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\CvT Database\input\administration_route\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAC1A73-DABF-47A5-A7BF-2935AD91A874}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9404AC60-8135-40F3-82BE-05C0A22F6972}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4908" yWindow="1332" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5568" yWindow="1740" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>administration_route_original</t>
   </si>
@@ -98,6 +98,21 @@
   </si>
   <si>
     <t>inhalation (nose only)</t>
+  </si>
+  <si>
+    <t>iv</t>
+  </si>
+  <si>
+    <t>oral</t>
+  </si>
+  <si>
+    <t>dermal</t>
+  </si>
+  <si>
+    <t>inhalation</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -487,10 +502,13 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -504,120 +522,192 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>